<commit_message>
added more names to map in dict
</commit_message>
<xml_diff>
--- a/names_dict.xlsx
+++ b/names_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lionel/Library/Mobile Documents/com~apple~CloudDocs/Capstone Project/SeaMoney/Capstone Github/Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C13F30-783D-0647-9D38-54AC4177F0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D19849-4D0C-7E47-A9BA-605CDF35EB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="28300" xr2:uid="{D3638201-87CB-CB41-AA34-3FB2B19DD51E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="259">
   <si>
     <t>gan</t>
   </si>
@@ -799,6 +799,18 @@
   </si>
   <si>
     <t>mohd., mohd, muhd, mohamad, mohammad, mohamed, mohammed, mohamat, muhamat, muhamed, muhamad, muhamed,  muhammed, muhammad</t>
+  </si>
+  <si>
+    <t>hassan</t>
+  </si>
+  <si>
+    <t>hasan</t>
+  </si>
+  <si>
+    <t>hussein</t>
+  </si>
+  <si>
+    <t>hussen, husein, hussain, husain</t>
   </si>
 </sst>
 </file>
@@ -1159,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6BC7BC9-3BD1-4247-A5C2-8F44BC5E9BC5}">
-  <dimension ref="A1:B129"/>
+  <dimension ref="A1:B131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="H130" sqref="H130"/>
+      <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2199,6 +2211,22 @@
         <v>254</v>
       </c>
     </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>255</v>
+      </c>
+      <c r="B130" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>257</v>
+      </c>
+      <c r="B131" t="s">
+        <v>258</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>